<commit_message>
fix mehrere papiermacher idns
</commit_message>
<xml_diff>
--- a/raw/riesaufdrucke.xlsx
+++ b/raw/riesaufdrucke.xlsx
@@ -388,7 +388,7 @@
     <t xml:space="preserve">18XX</t>
   </si>
   <si>
-    <t xml:space="preserve">18XX (Wirkungszeit des Papiermachers</t>
+    <t xml:space="preserve">18XX (Wirkungszeit des Papiermachers)</t>
   </si>
   <si>
     <t xml:space="preserve">Franz Leopold Fischer</t>
@@ -4282,10 +4282,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="U1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
-      <selection pane="bottomLeft" activeCell="Y9" activeCellId="0" sqref="Y9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15394,7 +15394,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="50.14"/>
   </cols>

</xml_diff>